<commit_message>
Changing Hardware for 2019
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2019.xlsx
+++ b/Kilroy Equipment List 2019.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="10590" windowHeight="5790"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="10596" windowHeight="5796"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$101</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -250,9 +250,6 @@
     <t>Speed Controllers (Type)</t>
   </si>
   <si>
-    <t>intakeDeployArm</t>
-  </si>
-  <si>
     <t>pdp</t>
   </si>
   <si>
@@ -482,6 +479,9 @@
   </si>
   <si>
     <t>USB Camera (USB 1)</t>
+  </si>
+  <si>
+    <t>armMotor</t>
   </si>
 </sst>
 </file>
@@ -1218,20 +1218,20 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M108" sqref="M108"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="53" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" style="53" customWidth="1"/>
-    <col min="3" max="3" width="50.7109375" style="53" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" style="53" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" style="53" customWidth="1"/>
+    <col min="3" max="3" width="50.6640625" style="53" customWidth="1"/>
     <col min="4" max="4" width="21" style="54" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" style="56" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" style="53" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="53"/>
-    <col min="8" max="8" width="11.140625" style="53" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="53"/>
+    <col min="5" max="5" width="18.109375" style="56" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" style="53" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="53"/>
+    <col min="8" max="8" width="11.109375" style="53" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="53"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1">
@@ -1243,7 +1243,7 @@
       <c r="D1" s="67"/>
       <c r="E1" s="67"/>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" ht="25.5">
+    <row r="2" spans="1:8" s="1" customFormat="1" ht="26.4">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
@@ -1260,7 +1260,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="1" customFormat="1" ht="13.15" customHeight="1">
+    <row r="3" spans="1:8" s="1" customFormat="1" ht="13.2" customHeight="1">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="66" t="s">
@@ -1289,39 +1289,39 @@
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="25" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D6" s="26" t="s">
         <v>75</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="34" customFormat="1">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>77</v>
+        <v>154</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1">
       <c r="A8" s="33"/>
       <c r="B8" s="33"/>
       <c r="C8" s="48" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D8" s="59" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E8" s="50" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
@@ -1341,13 +1341,13 @@
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E10" s="27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F10" s="12"/>
       <c r="G10" s="12"/>
@@ -1357,39 +1357,39 @@
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="28" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="1" customFormat="1">
       <c r="A12" s="13"/>
       <c r="B12" s="13"/>
       <c r="C12" s="22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E12" s="43" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="1" customFormat="1">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="28" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="1" customFormat="1">
@@ -1427,7 +1427,7 @@
       <c r="D18" s="63"/>
       <c r="E18" s="64"/>
     </row>
-    <row r="19" spans="1:8" s="1" customFormat="1" ht="13.15" customHeight="1">
+    <row r="19" spans="1:8" s="1" customFormat="1" ht="13.2" customHeight="1">
       <c r="A19" s="17"/>
       <c r="B19" s="17"/>
       <c r="C19" s="68" t="s">
@@ -1442,39 +1442,39 @@
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="D20" s="31" t="s">
-        <v>122</v>
-      </c>
       <c r="E20" s="32" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="1" customFormat="1">
       <c r="A21" s="51"/>
       <c r="B21" s="51"/>
       <c r="C21" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D21" s="26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E21" s="43" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="1" customFormat="1">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="28" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D22" s="31" t="s">
         <v>58</v>
       </c>
       <c r="E22" s="32" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F22" s="12"/>
       <c r="G22" s="12"/>
@@ -1571,163 +1571,163 @@
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E31" s="32" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="1" customFormat="1">
       <c r="A32" s="13"/>
       <c r="B32" s="13"/>
       <c r="C32" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D32" s="44" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E32" s="43" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" s="1" customFormat="1" ht="25.5">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="1" customFormat="1" ht="26.4">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="28" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D33" s="31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E33" s="32" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="1" customFormat="1" ht="25.5">
+    <row r="34" spans="1:5" s="1" customFormat="1" ht="26.4">
       <c r="A34" s="13"/>
       <c r="B34" s="13"/>
       <c r="C34" s="14" t="s">
         <v>56</v>
       </c>
       <c r="D34" s="44" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E34" s="43" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="1" customFormat="1">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D35" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E35" s="32" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="1" customFormat="1">
       <c r="A36" s="13"/>
       <c r="B36" s="13"/>
       <c r="C36" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D36" s="44" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E36" s="43" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="1" customFormat="1">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D37" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="E37" s="32" t="s">
         <v>127</v>
       </c>
-      <c r="D37" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="E37" s="32" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" s="1" customFormat="1" ht="25.5">
+    </row>
+    <row r="38" spans="1:5" s="1" customFormat="1" ht="26.4">
       <c r="A38" s="8"/>
       <c r="B38" s="8"/>
       <c r="C38" s="25" t="s">
         <v>39</v>
       </c>
       <c r="D38" s="60" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E38" s="27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="1" customFormat="1">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D39" s="31" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E39" s="32" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A40" s="13"/>
       <c r="B40" s="13"/>
       <c r="C40" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D40" s="44" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E40" s="43" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" s="18" customFormat="1" ht="13.15" customHeight="1">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" s="18" customFormat="1" ht="13.2" customHeight="1">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="28" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D41" s="6"/>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:5" s="1" customFormat="1" ht="13.15" customHeight="1">
+    <row r="42" spans="1:5" s="1" customFormat="1" ht="13.2" customHeight="1">
       <c r="A42" s="8"/>
       <c r="B42" s="8"/>
       <c r="C42" s="9"/>
       <c r="D42" s="10"/>
       <c r="E42" s="11"/>
     </row>
-    <row r="43" spans="1:5" s="18" customFormat="1" ht="13.15" customHeight="1">
+    <row r="43" spans="1:5" s="18" customFormat="1" ht="13.2" customHeight="1">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="5"/>
       <c r="D43" s="6"/>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="1:5" s="18" customFormat="1" ht="13.15" customHeight="1">
+    <row r="44" spans="1:5" s="18" customFormat="1" ht="13.2" customHeight="1">
       <c r="A44" s="13"/>
       <c r="B44" s="13"/>
       <c r="C44" s="14"/>
       <c r="D44" s="15"/>
       <c r="E44" s="16"/>
     </row>
-    <row r="45" spans="1:5" s="1" customFormat="1" ht="13.15" customHeight="1">
+    <row r="45" spans="1:5" s="1" customFormat="1" ht="13.2" customHeight="1">
       <c r="A45" s="17"/>
       <c r="B45" s="17"/>
       <c r="C45" s="66" t="s">
@@ -1780,7 +1780,7 @@
       <c r="D49" s="10"/>
       <c r="E49" s="11"/>
     </row>
-    <row r="50" spans="1:5" s="1" customFormat="1" ht="13.15" customHeight="1">
+    <row r="50" spans="1:5" s="1" customFormat="1" ht="13.2" customHeight="1">
       <c r="A50" s="17"/>
       <c r="B50" s="17"/>
       <c r="C50" s="66" t="s">
@@ -1791,11 +1791,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="18" customFormat="1" ht="13.15" customHeight="1">
+    <row r="51" spans="1:5" s="18" customFormat="1" ht="13.2" customHeight="1">
       <c r="A51" s="19"/>
       <c r="B51" s="19"/>
       <c r="C51" s="45" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D51" s="24" t="s">
         <v>40</v>
@@ -1808,10 +1808,10 @@
       <c r="A52" s="8"/>
       <c r="B52" s="8"/>
       <c r="C52" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D52" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E52" s="27" t="s">
         <v>43</v>
@@ -1821,10 +1821,10 @@
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="D53" s="31" t="s">
         <v>115</v>
-      </c>
-      <c r="D53" s="31" t="s">
-        <v>116</v>
       </c>
       <c r="E53" s="32" t="s">
         <v>42</v>
@@ -1851,25 +1851,25 @@
       <c r="D56" s="26"/>
       <c r="E56" s="27"/>
     </row>
-    <row r="57" spans="1:5" s="1" customFormat="1" ht="13.15" customHeight="1">
+    <row r="57" spans="1:5" s="1" customFormat="1" ht="13.2" customHeight="1">
       <c r="A57" s="17"/>
       <c r="B57" s="17"/>
       <c r="C57" s="66" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D57" s="66"/>
       <c r="E57" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="58" spans="1:5" s="18" customFormat="1" ht="13.15" customHeight="1">
+    <row r="58" spans="1:5" s="18" customFormat="1" ht="13.2" customHeight="1">
       <c r="A58" s="19"/>
       <c r="B58" s="19"/>
       <c r="C58" s="45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D58" s="24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E58" s="46"/>
     </row>
@@ -1909,49 +1909,49 @@
       <c r="A63" s="19"/>
       <c r="B63" s="19"/>
       <c r="C63" s="65" t="s">
+        <v>93</v>
+      </c>
+      <c r="D63" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="E63" s="32" t="s">
         <v>94</v>
-      </c>
-      <c r="D63" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="E63" s="32" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="64" spans="1:5" s="1" customFormat="1">
       <c r="A64" s="8"/>
       <c r="B64" s="8"/>
       <c r="C64" s="25" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D64" s="26"/>
       <c r="E64" s="27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="65" spans="1:8" s="1" customFormat="1">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="28" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D65" s="31"/>
       <c r="E65" s="32" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="66" spans="1:8" s="1" customFormat="1">
       <c r="A66" s="8"/>
       <c r="B66" s="8"/>
       <c r="C66" s="25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D66" s="26"/>
       <c r="E66" s="27" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" s="35" customFormat="1" ht="13.15" customHeight="1">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" s="35" customFormat="1" ht="13.2" customHeight="1">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="C67" s="5"/>
@@ -1978,7 +1978,7 @@
         <v>60</v>
       </c>
       <c r="D69" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E69" s="11" t="s">
         <v>50</v>
@@ -1998,7 +1998,7 @@
       <c r="D71" s="10"/>
       <c r="E71" s="11"/>
     </row>
-    <row r="72" spans="1:8" s="35" customFormat="1" ht="13.15" customHeight="1">
+    <row r="72" spans="1:8" s="35" customFormat="1" ht="13.2" customHeight="1">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
       <c r="C72" s="5"/>
@@ -2129,7 +2129,7 @@
       <c r="D84" s="31"/>
       <c r="E84" s="32"/>
     </row>
-    <row r="85" spans="1:6" s="1" customFormat="1" ht="13.15" customHeight="1">
+    <row r="85" spans="1:6" s="1" customFormat="1" ht="13.2" customHeight="1">
       <c r="A85" s="13"/>
       <c r="B85" s="8"/>
       <c r="C85" s="29"/>
@@ -2144,7 +2144,7 @@
       <c r="D86" s="31"/>
       <c r="E86" s="32"/>
     </row>
-    <row r="87" spans="1:6" s="1" customFormat="1" ht="13.15" customHeight="1">
+    <row r="87" spans="1:6" s="1" customFormat="1" ht="13.2" customHeight="1">
       <c r="A87" s="13"/>
       <c r="B87" s="8"/>
       <c r="C87" s="22"/>
@@ -2174,7 +2174,7 @@
       <c r="D90" s="31"/>
       <c r="E90" s="32"/>
     </row>
-    <row r="91" spans="1:6" s="1" customFormat="1" ht="13.15" customHeight="1">
+    <row r="91" spans="1:6" s="1" customFormat="1" ht="13.2" customHeight="1">
       <c r="A91" s="13"/>
       <c r="B91" s="8"/>
       <c r="C91" s="22"/>
@@ -2189,7 +2189,7 @@
       <c r="D92" s="6"/>
       <c r="E92" s="32"/>
     </row>
-    <row r="93" spans="1:6" s="1" customFormat="1" ht="13.15" customHeight="1">
+    <row r="93" spans="1:6" s="1" customFormat="1" ht="13.2" customHeight="1">
       <c r="A93" s="13"/>
       <c r="B93" s="8"/>
       <c r="C93" s="22"/>
@@ -2219,7 +2219,7 @@
       <c r="D96" s="31"/>
       <c r="E96" s="32"/>
     </row>
-    <row r="97" spans="1:7" s="1" customFormat="1" ht="13.15" customHeight="1">
+    <row r="97" spans="1:7" s="1" customFormat="1" ht="13.2" customHeight="1">
       <c r="A97" s="13"/>
       <c r="B97" s="8"/>
       <c r="C97" s="22"/>
@@ -2300,17 +2300,17 @@
         <v>7</v>
       </c>
       <c r="E104" s="32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="105" spans="1:7" s="1" customFormat="1">
       <c r="A105" s="13"/>
       <c r="B105" s="13"/>
       <c r="C105" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D105" s="26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E105" s="43" t="s">
         <v>19</v>
@@ -2385,10 +2385,10 @@
       <c r="A111" s="13"/>
       <c r="B111" s="13"/>
       <c r="C111" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D111" s="15" t="s">
         <v>105</v>
-      </c>
-      <c r="D111" s="15" t="s">
-        <v>106</v>
       </c>
       <c r="E111" s="16" t="s">
         <v>19</v>
@@ -2398,10 +2398,10 @@
       <c r="A112" s="4"/>
       <c r="B112" s="4"/>
       <c r="C112" s="28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D112" s="31" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E112" s="32"/>
     </row>
@@ -2431,7 +2431,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="115" spans="1:5" s="1" customFormat="1" ht="25.5">
+    <row r="115" spans="1:5" s="1" customFormat="1" ht="26.4">
       <c r="A115" s="13"/>
       <c r="B115" s="13"/>
       <c r="C115" s="14" t="s">
@@ -2448,10 +2448,10 @@
       <c r="A116" s="4"/>
       <c r="B116" s="4"/>
       <c r="C116" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="D116" s="31" t="s">
         <v>103</v>
-      </c>
-      <c r="D116" s="31" t="s">
-        <v>104</v>
       </c>
       <c r="E116" s="32" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Changed armIR to armBallDetector
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2019.xlsx
+++ b/Kilroy Equipment List 2019.xlsx
@@ -193,9 +193,6 @@
     <t>PCM Port</t>
   </si>
   <si>
-    <t>armIR</t>
-  </si>
-  <si>
     <t>Kilroy Equipment List (2019)</t>
   </si>
   <si>
@@ -482,6 +479,9 @@
   </si>
   <si>
     <t>armMotor</t>
+  </si>
+  <si>
+    <t>armBallDetector</t>
   </si>
 </sst>
 </file>
@@ -1217,8 +1217,8 @@
   <dimension ref="A1:H241"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D66" sqref="D66"/>
+      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -1236,7 +1236,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="67" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B1" s="67"/>
       <c r="C1" s="67"/>
@@ -1264,7 +1264,7 @@
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="66" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D3" s="66"/>
       <c r="E3" s="3" t="s">
@@ -1289,39 +1289,39 @@
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="34" customFormat="1">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="28" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1">
       <c r="A8" s="33"/>
       <c r="B8" s="33"/>
       <c r="C8" s="48" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D8" s="59" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E8" s="50" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
@@ -1341,13 +1341,13 @@
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E10" s="27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F10" s="12"/>
       <c r="G10" s="12"/>
@@ -1357,39 +1357,39 @@
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="1" customFormat="1">
       <c r="A12" s="13"/>
       <c r="B12" s="13"/>
       <c r="C12" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E12" s="43" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="1" customFormat="1">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="28" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="1" customFormat="1">
@@ -1442,39 +1442,39 @@
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="D20" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="D20" s="31" t="s">
-        <v>121</v>
-      </c>
       <c r="E20" s="32" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="1" customFormat="1">
       <c r="A21" s="51"/>
       <c r="B21" s="51"/>
       <c r="C21" s="25" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D21" s="26" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E21" s="43" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="1" customFormat="1">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>58</v>
+        <v>154</v>
       </c>
       <c r="E22" s="32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F22" s="12"/>
       <c r="G22" s="12"/>
@@ -1545,65 +1545,65 @@
       <c r="A29" s="42"/>
       <c r="B29" s="42"/>
       <c r="C29" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="E29" s="32" t="s">
         <v>62</v>
-      </c>
-      <c r="D29" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="E29" s="32" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="1" customFormat="1">
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
       <c r="C30" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D30" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="E30" s="43" t="s">
         <v>64</v>
-      </c>
-      <c r="E30" s="43" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:8" s="1" customFormat="1">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E31" s="32" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="1" customFormat="1">
       <c r="A32" s="13"/>
       <c r="B32" s="13"/>
       <c r="C32" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D32" s="44" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E32" s="43" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="1" customFormat="1" ht="25.5">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="28" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D33" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E33" s="32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="1" customFormat="1" ht="25.5">
@@ -1613,49 +1613,49 @@
         <v>56</v>
       </c>
       <c r="D34" s="44" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E34" s="43" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="1" customFormat="1">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D35" s="31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E35" s="32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="1" customFormat="1">
       <c r="A36" s="13"/>
       <c r="B36" s="13"/>
       <c r="C36" s="22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D36" s="44" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E36" s="43" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="1" customFormat="1">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D37" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="E37" s="32" t="s">
         <v>126</v>
-      </c>
-      <c r="D37" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="E37" s="32" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="1" customFormat="1" ht="25.5">
@@ -1665,43 +1665,43 @@
         <v>39</v>
       </c>
       <c r="D38" s="60" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E38" s="27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="1" customFormat="1">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D39" s="31" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E39" s="32" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A40" s="13"/>
       <c r="B40" s="13"/>
       <c r="C40" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D40" s="44" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E40" s="43" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="41" spans="1:5" s="18" customFormat="1" ht="13.15" customHeight="1">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D41" s="6"/>
       <c r="E41" s="7"/>
@@ -1795,7 +1795,7 @@
       <c r="A51" s="19"/>
       <c r="B51" s="19"/>
       <c r="C51" s="45" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D51" s="24" t="s">
         <v>40</v>
@@ -1808,10 +1808,10 @@
       <c r="A52" s="8"/>
       <c r="B52" s="8"/>
       <c r="C52" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D52" s="26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E52" s="27" t="s">
         <v>43</v>
@@ -1821,10 +1821,10 @@
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="D53" s="31" t="s">
         <v>114</v>
-      </c>
-      <c r="D53" s="31" t="s">
-        <v>115</v>
       </c>
       <c r="E53" s="32" t="s">
         <v>42</v>
@@ -1855,7 +1855,7 @@
       <c r="A57" s="17"/>
       <c r="B57" s="17"/>
       <c r="C57" s="66" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D57" s="66"/>
       <c r="E57" s="3" t="s">
@@ -1866,10 +1866,10 @@
       <c r="A58" s="19"/>
       <c r="B58" s="19"/>
       <c r="C58" s="45" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D58" s="24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E58" s="46"/>
     </row>
@@ -1909,46 +1909,46 @@
       <c r="A63" s="19"/>
       <c r="B63" s="19"/>
       <c r="C63" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="D63" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="E63" s="32" t="s">
         <v>93</v>
-      </c>
-      <c r="D63" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="E63" s="32" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="64" spans="1:5" s="1" customFormat="1">
       <c r="A64" s="8"/>
       <c r="B64" s="8"/>
       <c r="C64" s="25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D64" s="26"/>
       <c r="E64" s="27" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="65" spans="1:8" s="1" customFormat="1">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="28" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D65" s="31"/>
       <c r="E65" s="32" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="66" spans="1:8" s="1" customFormat="1">
       <c r="A66" s="8"/>
       <c r="B66" s="8"/>
       <c r="C66" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D66" s="26"/>
       <c r="E66" s="27" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="67" spans="1:8" s="35" customFormat="1" ht="13.15" customHeight="1">
@@ -1975,10 +1975,10 @@
       <c r="A69" s="8"/>
       <c r="B69" s="8"/>
       <c r="C69" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D69" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E69" s="11" t="s">
         <v>50</v>
@@ -2300,17 +2300,17 @@
         <v>7</v>
       </c>
       <c r="E104" s="32" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="105" spans="1:7" s="1" customFormat="1">
       <c r="A105" s="13"/>
       <c r="B105" s="13"/>
       <c r="C105" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D105" s="26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E105" s="43" t="s">
         <v>19</v>
@@ -2320,10 +2320,10 @@
       <c r="A106" s="4"/>
       <c r="B106" s="4"/>
       <c r="C106" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D106" s="31" t="s">
         <v>69</v>
-      </c>
-      <c r="D106" s="31" t="s">
-        <v>70</v>
       </c>
       <c r="E106" s="32" t="s">
         <v>19</v>
@@ -2385,10 +2385,10 @@
       <c r="A111" s="13"/>
       <c r="B111" s="13"/>
       <c r="C111" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D111" s="15" t="s">
         <v>104</v>
-      </c>
-      <c r="D111" s="15" t="s">
-        <v>105</v>
       </c>
       <c r="E111" s="16" t="s">
         <v>19</v>
@@ -2398,10 +2398,10 @@
       <c r="A112" s="4"/>
       <c r="B112" s="4"/>
       <c r="C112" s="28" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D112" s="31" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E112" s="32"/>
     </row>
@@ -2409,10 +2409,10 @@
       <c r="A113" s="13"/>
       <c r="B113" s="13"/>
       <c r="C113" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D113" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E113" s="16" t="s">
         <v>19</v>
@@ -2422,10 +2422,10 @@
       <c r="A114" s="4"/>
       <c r="B114" s="4"/>
       <c r="C114" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D114" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E114" s="32" t="s">
         <v>19</v>
@@ -2435,10 +2435,10 @@
       <c r="A115" s="13"/>
       <c r="B115" s="13"/>
       <c r="C115" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D115" s="44" t="s">
         <v>73</v>
-      </c>
-      <c r="D115" s="44" t="s">
-        <v>74</v>
       </c>
       <c r="E115" s="22" t="s">
         <v>19</v>
@@ -2448,10 +2448,10 @@
       <c r="A116" s="4"/>
       <c r="B116" s="4"/>
       <c r="C116" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="D116" s="31" t="s">
         <v>102</v>
-      </c>
-      <c r="D116" s="31" t="s">
-        <v>103</v>
       </c>
       <c r="E116" s="32" t="s">
         <v>19</v>

</xml_diff>